<commit_message>
update(template): add product upload template file
</commit_message>
<xml_diff>
--- a/stocky-api/src/main/resources/downloads/ProductUploadTemplate.xlsx
+++ b/stocky-api/src/main/resources/downloads/ProductUploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Development/java-projects/stocky/stocky-api/src/main/resources/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8E6202-07F1-CB4A-A6E7-6CA85A51171F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92886C98-94D6-1B49-A44D-276382009B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Category</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>ServiceOrProduct</t>
-  </si>
-  <si>
-    <t>LowStockPoint</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -468,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE505DCF-D03B-E749-931E-022DA2288EDF}">
-  <dimension ref="B2:E27"/>
+  <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,127 +478,130 @@
     <col min="4" max="4" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="26" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
@@ -639,16 +639,6 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -657,10 +647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView zoomScale="68" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,14 +665,13 @@
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.83203125" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,13 +717,10 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>